<commit_message>
ready to test the impact of flips
</commit_message>
<xml_diff>
--- a/error/size/image_size.xlsx
+++ b/error/size/image_size.xlsx
@@ -160,12 +160,12 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1047,6 +1047,20 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
         <c:title>
           <c:tx>
             <c:rich>
@@ -2315,7 +2329,7 @@
   <dimension ref="A1:V71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AE49" sqref="AE49"/>
+      <selection activeCell="AE27" sqref="AE27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2326,7 +2340,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="12" t="s">
         <v>12</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -2358,7 +2372,7 @@
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A2" s="9"/>
+      <c r="A2" s="12"/>
       <c r="B2" s="2">
         <v>0</v>
       </c>
@@ -2417,7 +2431,7 @@
       <c r="V2" s="8"/>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A3" s="9"/>
+      <c r="A3" s="12"/>
       <c r="B3" s="2">
         <v>1</v>
       </c>
@@ -2449,7 +2463,7 @@
       <c r="M3" s="8">
         <v>0</v>
       </c>
-      <c r="N3" s="10">
+      <c r="N3" s="9">
         <v>0.859130859375</v>
       </c>
       <c r="O3">
@@ -2476,7 +2490,7 @@
       <c r="V3" s="8"/>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A4" s="9"/>
+      <c r="A4" s="12"/>
       <c r="B4" s="2">
         <v>2</v>
       </c>
@@ -2508,7 +2522,7 @@
       <c r="M4" s="8">
         <v>1</v>
       </c>
-      <c r="N4" s="10">
+      <c r="N4" s="9">
         <v>0.730712890625</v>
       </c>
       <c r="O4">
@@ -2535,7 +2549,7 @@
       <c r="V4" s="8"/>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A5" s="9"/>
+      <c r="A5" s="12"/>
       <c r="B5" s="2">
         <v>3</v>
       </c>
@@ -2567,7 +2581,7 @@
       <c r="M5" s="8">
         <v>2</v>
       </c>
-      <c r="N5" s="10">
+      <c r="N5" s="9">
         <v>0.325439453125</v>
       </c>
       <c r="O5">
@@ -2594,7 +2608,7 @@
       <c r="V5" s="8"/>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A6" s="9"/>
+      <c r="A6" s="12"/>
       <c r="B6" s="2">
         <v>4</v>
       </c>
@@ -2626,7 +2640,7 @@
       <c r="M6" s="8">
         <v>3</v>
       </c>
-      <c r="N6" s="10">
+      <c r="N6" s="9">
         <v>0.68115234375</v>
       </c>
       <c r="O6">
@@ -2653,7 +2667,7 @@
       <c r="V6" s="8"/>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A7" s="9"/>
+      <c r="A7" s="12"/>
       <c r="B7" s="2">
         <v>5</v>
       </c>
@@ -2685,7 +2699,7 @@
       <c r="M7" s="8">
         <v>4</v>
       </c>
-      <c r="N7" s="10">
+      <c r="N7" s="9">
         <v>0.873291015625</v>
       </c>
       <c r="O7">
@@ -2712,7 +2726,7 @@
       <c r="V7" s="8"/>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A8" s="9"/>
+      <c r="A8" s="12"/>
       <c r="B8" s="2">
         <v>6</v>
       </c>
@@ -2744,7 +2758,7 @@
       <c r="M8" s="8">
         <v>5</v>
       </c>
-      <c r="N8" s="10">
+      <c r="N8" s="9">
         <v>0.977783203125</v>
       </c>
       <c r="O8">
@@ -2774,7 +2788,7 @@
       <c r="M9" s="8">
         <v>6</v>
       </c>
-      <c r="N9" s="10">
+      <c r="N9" s="9">
         <v>0.49755859375</v>
       </c>
       <c r="O9">
@@ -2801,7 +2815,7 @@
       <c r="V9" s="8"/>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="12" t="s">
         <v>1</v>
       </c>
       <c r="B10" s="2" t="s">
@@ -2831,19 +2845,19 @@
       <c r="K10" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="M10" s="12"/>
-      <c r="N10" s="12"/>
-      <c r="O10" s="12"/>
-      <c r="P10" s="12"/>
-      <c r="Q10" s="12"/>
-      <c r="R10" s="12"/>
-      <c r="S10" s="12"/>
-      <c r="T10" s="12"/>
-      <c r="U10" s="12"/>
+      <c r="M10" s="11"/>
+      <c r="N10" s="11"/>
+      <c r="O10" s="11"/>
+      <c r="P10" s="11"/>
+      <c r="Q10" s="11"/>
+      <c r="R10" s="11"/>
+      <c r="S10" s="11"/>
+      <c r="T10" s="11"/>
+      <c r="U10" s="11"/>
       <c r="V10" s="8"/>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A11" s="9"/>
+      <c r="A11" s="12"/>
       <c r="B11" s="2">
         <v>0</v>
       </c>
@@ -2875,7 +2889,7 @@
       <c r="M11" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="N11" s="10">
+      <c r="N11" s="9">
         <f>AVERAGE(N3:N9)</f>
         <v>0.7064383370535714</v>
       </c>
@@ -2884,7 +2898,7 @@
         <v>0.79951769067415335</v>
       </c>
       <c r="P11">
-        <f t="shared" ref="P11:S11" si="0">AVERAGE(P3:P9)</f>
+        <f t="shared" ref="P11:R11" si="0">AVERAGE(P3:P9)</f>
         <v>0.77198909663300952</v>
       </c>
       <c r="Q11">
@@ -2895,7 +2909,7 @@
         <f t="shared" si="0"/>
         <v>0.83616937079540954</v>
       </c>
-      <c r="S11" s="11">
+      <c r="S11" s="10">
         <f>AVERAGE(S3:S9)</f>
         <v>0.88817001180637534</v>
       </c>
@@ -2903,14 +2917,14 @@
         <f>AVERAGE(T3:T9)</f>
         <v>0.92107003000559418</v>
       </c>
-      <c r="U11" s="11">
+      <c r="U11" s="10">
         <f>AVERAGE(U3:U9)</f>
         <v>0.86065329922056288</v>
       </c>
       <c r="V11" s="8"/>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A12" s="9"/>
+      <c r="A12" s="12"/>
       <c r="B12" s="2">
         <v>1</v>
       </c>
@@ -2942,7 +2956,7 @@
       <c r="M12" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="N12" s="10">
+      <c r="N12" s="9">
         <f>MEDIAN(N3:N9)</f>
         <v>0.730712890625</v>
       </c>
@@ -2962,7 +2976,7 @@
         <f t="shared" si="1"/>
         <v>0.95506309633733455</v>
       </c>
-      <c r="S12" s="11">
+      <c r="S12" s="10">
         <f t="shared" si="1"/>
         <v>0.99041322314049585</v>
       </c>
@@ -2970,14 +2984,14 @@
         <f t="shared" si="1"/>
         <v>0.99359202563189752</v>
       </c>
-      <c r="U12" s="11">
+      <c r="U12" s="10">
         <f>MEDIAN(U3:U9)</f>
         <v>0.985006247396918</v>
       </c>
       <c r="V12" s="8"/>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A13" s="9"/>
+      <c r="A13" s="12"/>
       <c r="B13" s="2">
         <v>2</v>
       </c>
@@ -3009,7 +3023,7 @@
       <c r="M13" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="N13" s="10">
+      <c r="N13" s="9">
         <f>LARGE(N3:N9,1)</f>
         <v>0.977783203125</v>
       </c>
@@ -3044,7 +3058,7 @@
       <c r="V13" s="8"/>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A14" s="9"/>
+      <c r="A14" s="12"/>
       <c r="B14" s="2">
         <v>3</v>
       </c>
@@ -3076,7 +3090,7 @@
       <c r="M14" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="N14" s="10">
+      <c r="N14" s="9">
         <f>SMALL(N3:N9,1)</f>
         <v>0.325439453125</v>
       </c>
@@ -3096,7 +3110,7 @@
         <f t="shared" si="4"/>
         <v>0.42905509387503848</v>
       </c>
-      <c r="S14" s="11">
+      <c r="S14" s="10">
         <f t="shared" si="4"/>
         <v>0.57289256198347105</v>
       </c>
@@ -3104,14 +3118,14 @@
         <f t="shared" si="4"/>
         <v>0.59166963332146671</v>
       </c>
-      <c r="U14" s="11">
+      <c r="U14" s="10">
         <f t="shared" ref="U14" si="5">SMALL(U3:U9,1)</f>
         <v>0.54977092877967515</v>
       </c>
       <c r="V14" s="8"/>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A15" s="9"/>
+      <c r="A15" s="12"/>
       <c r="B15" s="2">
         <v>4</v>
       </c>
@@ -3140,10 +3154,10 @@
         <f>G15/SUM(C15:I15)</f>
         <v>0.77651801461325276</v>
       </c>
-      <c r="R15" s="10"/>
+      <c r="R15" s="9"/>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A16" s="9"/>
+      <c r="A16" s="12"/>
       <c r="B16" s="2">
         <v>5</v>
       </c>
@@ -3172,10 +3186,10 @@
         <f>H16/SUM(C16:I16)</f>
         <v>0.91836734693877553</v>
       </c>
-      <c r="R16" s="10"/>
+      <c r="R16" s="9"/>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A17" s="9"/>
+      <c r="A17" s="12"/>
       <c r="B17" s="2">
         <v>6</v>
       </c>
@@ -3204,13 +3218,13 @@
         <f>I17/SUM(C17:I17)</f>
         <v>0.96371882086167804</v>
       </c>
-      <c r="R17" s="10"/>
+      <c r="R17" s="9"/>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="R18" s="10"/>
+      <c r="R18" s="9"/>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A19" s="9" t="s">
+      <c r="A19" s="12" t="s">
         <v>7</v>
       </c>
       <c r="B19" s="2" t="s">
@@ -3240,10 +3254,10 @@
       <c r="K19" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="R19" s="10"/>
+      <c r="R19" s="9"/>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A20" s="9"/>
+      <c r="A20" s="12"/>
       <c r="B20" s="2">
         <v>0</v>
       </c>
@@ -3274,10 +3288,10 @@
       </c>
       <c r="M20" s="1"/>
       <c r="O20" s="1"/>
-      <c r="R20" s="10"/>
+      <c r="R20" s="9"/>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A21" s="9"/>
+      <c r="A21" s="12"/>
       <c r="B21" s="2">
         <v>1</v>
       </c>
@@ -3306,10 +3320,10 @@
         <f>D21/SUM(C21:I21)</f>
         <v>0.91561408223595808</v>
       </c>
-      <c r="R21" s="10"/>
+      <c r="R21" s="9"/>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A22" s="9"/>
+      <c r="A22" s="12"/>
       <c r="B22" s="2">
         <v>2</v>
       </c>
@@ -3338,10 +3352,10 @@
         <f>E22/SUM(C22:I22)</f>
         <v>0.27250739048642836</v>
       </c>
-      <c r="R22" s="10"/>
+      <c r="R22" s="9"/>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A23" s="9"/>
+      <c r="A23" s="12"/>
       <c r="B23" s="2">
         <v>3</v>
       </c>
@@ -3372,10 +3386,10 @@
       </c>
       <c r="M23" s="1"/>
       <c r="O23" s="1"/>
-      <c r="R23" s="10"/>
+      <c r="R23" s="9"/>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A24" s="9"/>
+      <c r="A24" s="12"/>
       <c r="B24" s="2">
         <v>4</v>
       </c>
@@ -3404,10 +3418,10 @@
         <f>G24/SUM(C24:I24)</f>
         <v>0.80274119860252624</v>
       </c>
-      <c r="R24" s="10"/>
+      <c r="R24" s="9"/>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A25" s="9"/>
+      <c r="A25" s="12"/>
       <c r="B25" s="2">
         <v>5</v>
       </c>
@@ -3436,10 +3450,10 @@
         <f>H25/SUM(C25:I25)</f>
         <v>0.8844396667562483</v>
       </c>
-      <c r="R25" s="10"/>
+      <c r="R25" s="9"/>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A26" s="9"/>
+      <c r="A26" s="12"/>
       <c r="B26" s="2">
         <v>6</v>
       </c>
@@ -3470,7 +3484,7 @@
       </c>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A28" s="9" t="s">
+      <c r="A28" s="12" t="s">
         <v>8</v>
       </c>
       <c r="B28" s="2" t="s">
@@ -3502,7 +3516,7 @@
       </c>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A29" s="9"/>
+      <c r="A29" s="12"/>
       <c r="B29" s="2">
         <v>0</v>
       </c>
@@ -3535,7 +3549,7 @@
       <c r="O29" s="1"/>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A30" s="9"/>
+      <c r="A30" s="12"/>
       <c r="B30" s="2">
         <v>1</v>
       </c>
@@ -3566,7 +3580,7 @@
       </c>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A31" s="9"/>
+      <c r="A31" s="12"/>
       <c r="B31" s="2">
         <v>2</v>
       </c>
@@ -3597,7 +3611,7 @@
       </c>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A32" s="9"/>
+      <c r="A32" s="12"/>
       <c r="B32" s="2">
         <v>3</v>
       </c>
@@ -3630,7 +3644,7 @@
       <c r="O32" s="1"/>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A33" s="9"/>
+      <c r="A33" s="12"/>
       <c r="B33" s="2">
         <v>4</v>
       </c>
@@ -3661,7 +3675,7 @@
       </c>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A34" s="9"/>
+      <c r="A34" s="12"/>
       <c r="B34" s="2">
         <v>5</v>
       </c>
@@ -3692,7 +3706,7 @@
       </c>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A35" s="9"/>
+      <c r="A35" s="12"/>
       <c r="B35" s="2">
         <v>6</v>
       </c>
@@ -3723,7 +3737,7 @@
       </c>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A37" s="9" t="s">
+      <c r="A37" s="12" t="s">
         <v>9</v>
       </c>
       <c r="B37" s="2" t="s">
@@ -3755,7 +3769,7 @@
       </c>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A38" s="9"/>
+      <c r="A38" s="12"/>
       <c r="B38" s="2">
         <v>0</v>
       </c>
@@ -3788,7 +3802,7 @@
       <c r="O38" s="1"/>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A39" s="9"/>
+      <c r="A39" s="12"/>
       <c r="B39" s="2">
         <v>1</v>
       </c>
@@ -3819,7 +3833,7 @@
       </c>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A40" s="9"/>
+      <c r="A40" s="12"/>
       <c r="B40" s="2">
         <v>2</v>
       </c>
@@ -3850,7 +3864,7 @@
       </c>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A41" s="9"/>
+      <c r="A41" s="12"/>
       <c r="B41" s="2">
         <v>3</v>
       </c>
@@ -3883,7 +3897,7 @@
       <c r="O41" s="1"/>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A42" s="9"/>
+      <c r="A42" s="12"/>
       <c r="B42" s="2">
         <v>4</v>
       </c>
@@ -3914,7 +3928,7 @@
       </c>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A43" s="9"/>
+      <c r="A43" s="12"/>
       <c r="B43" s="2">
         <v>5</v>
       </c>
@@ -3945,7 +3959,7 @@
       </c>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A44" s="9"/>
+      <c r="A44" s="12"/>
       <c r="B44" s="2">
         <v>6</v>
       </c>
@@ -3976,7 +3990,7 @@
       </c>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A46" s="9" t="s">
+      <c r="A46" s="12" t="s">
         <v>10</v>
       </c>
       <c r="B46" s="2" t="s">
@@ -4008,7 +4022,7 @@
       </c>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A47" s="9"/>
+      <c r="A47" s="12"/>
       <c r="B47" s="2">
         <v>0</v>
       </c>
@@ -4041,7 +4055,7 @@
       <c r="O47" s="1"/>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A48" s="9"/>
+      <c r="A48" s="12"/>
       <c r="B48" s="2">
         <v>1</v>
       </c>
@@ -4072,7 +4086,7 @@
       </c>
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A49" s="9"/>
+      <c r="A49" s="12"/>
       <c r="B49" s="2">
         <v>2</v>
       </c>
@@ -4103,7 +4117,7 @@
       </c>
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A50" s="9"/>
+      <c r="A50" s="12"/>
       <c r="B50" s="2">
         <v>3</v>
       </c>
@@ -4136,7 +4150,7 @@
       <c r="O50" s="1"/>
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A51" s="9"/>
+      <c r="A51" s="12"/>
       <c r="B51" s="2">
         <v>4</v>
       </c>
@@ -4167,7 +4181,7 @@
       </c>
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A52" s="9"/>
+      <c r="A52" s="12"/>
       <c r="B52" s="2">
         <v>5</v>
       </c>
@@ -4198,7 +4212,7 @@
       </c>
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A53" s="9"/>
+      <c r="A53" s="12"/>
       <c r="B53" s="2">
         <v>6</v>
       </c>
@@ -4229,7 +4243,7 @@
       </c>
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A55" s="9" t="s">
+      <c r="A55" s="12" t="s">
         <v>13</v>
       </c>
       <c r="B55" s="2" t="s">
@@ -4261,7 +4275,7 @@
       </c>
     </row>
     <row r="56" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A56" s="9"/>
+      <c r="A56" s="12"/>
       <c r="B56" s="2">
         <v>0</v>
       </c>
@@ -4294,7 +4308,7 @@
       <c r="O56" s="1"/>
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A57" s="9"/>
+      <c r="A57" s="12"/>
       <c r="B57" s="2">
         <v>1</v>
       </c>
@@ -4325,7 +4339,7 @@
       </c>
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A58" s="9"/>
+      <c r="A58" s="12"/>
       <c r="B58" s="2">
         <v>2</v>
       </c>
@@ -4356,7 +4370,7 @@
       </c>
     </row>
     <row r="59" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A59" s="9"/>
+      <c r="A59" s="12"/>
       <c r="B59" s="2">
         <v>3</v>
       </c>
@@ -4389,7 +4403,7 @@
       <c r="O59" s="1"/>
     </row>
     <row r="60" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A60" s="9"/>
+      <c r="A60" s="12"/>
       <c r="B60" s="2">
         <v>4</v>
       </c>
@@ -4420,7 +4434,7 @@
       </c>
     </row>
     <row r="61" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A61" s="9"/>
+      <c r="A61" s="12"/>
       <c r="B61" s="2">
         <v>5</v>
       </c>
@@ -4451,7 +4465,7 @@
       </c>
     </row>
     <row r="62" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A62" s="9"/>
+      <c r="A62" s="12"/>
       <c r="B62" s="2">
         <v>6</v>
       </c>
@@ -4482,7 +4496,7 @@
       </c>
     </row>
     <row r="64" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A64" s="9" t="s">
+      <c r="A64" s="12" t="s">
         <v>14</v>
       </c>
       <c r="B64" s="2" t="s">
@@ -4514,7 +4528,7 @@
       </c>
     </row>
     <row r="65" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A65" s="9"/>
+      <c r="A65" s="12"/>
       <c r="B65" s="2">
         <v>0</v>
       </c>
@@ -4547,7 +4561,7 @@
       <c r="O65" s="1"/>
     </row>
     <row r="66" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A66" s="9"/>
+      <c r="A66" s="12"/>
       <c r="B66" s="2">
         <v>1</v>
       </c>
@@ -4578,7 +4592,7 @@
       </c>
     </row>
     <row r="67" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A67" s="9"/>
+      <c r="A67" s="12"/>
       <c r="B67" s="2">
         <v>2</v>
       </c>
@@ -4609,7 +4623,7 @@
       </c>
     </row>
     <row r="68" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A68" s="9"/>
+      <c r="A68" s="12"/>
       <c r="B68" s="2">
         <v>3</v>
       </c>
@@ -4642,7 +4656,7 @@
       <c r="O68" s="1"/>
     </row>
     <row r="69" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A69" s="9"/>
+      <c r="A69" s="12"/>
       <c r="B69" s="2">
         <v>4</v>
       </c>
@@ -4673,7 +4687,7 @@
       </c>
     </row>
     <row r="70" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A70" s="9"/>
+      <c r="A70" s="12"/>
       <c r="B70" s="2">
         <v>5</v>
       </c>
@@ -4704,7 +4718,7 @@
       </c>
     </row>
     <row r="71" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A71" s="9"/>
+      <c r="A71" s="12"/>
       <c r="B71" s="2">
         <v>6</v>
       </c>

</xml_diff>